<commit_message>
Updated Comp 590 -173 Figure 27 & 32
</commit_message>
<xml_diff>
--- a/FinalProjectFigure27.xlsx
+++ b/FinalProjectFigure27.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vidyuthj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A07388-689F-C24F-BFCD-8CE0D64A0518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E8062A-BDD3-7D47-97D5-2748C39D5FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="26400" windowHeight="16480" xr2:uid="{93F4A4A9-9A46-7D43-9059-556CCE51DD7C}"/>
+    <workbookView xWindow="8540" yWindow="520" windowWidth="20260" windowHeight="16480" xr2:uid="{93F4A4A9-9A46-7D43-9059-556CCE51DD7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,17 +50,25 @@
     <t>Post Malone</t>
   </si>
   <si>
-    <t>Bad Bunny</t>
+    <t>Rihanna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,13 +91,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -271,7 +283,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23000000</c:v>
+                  <c:v>41400000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>80000000</c:v>
@@ -366,13 +378,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>49000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>14200000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,13 +473,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14700000</c:v>
+                  <c:v>32800000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>75000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30000000</c:v>
+                  <c:v>75000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,10 +568,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23200000</c:v>
+                  <c:v>29700000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24000000</c:v>
+                  <c:v>60000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45000000</c:v>
@@ -583,7 +595,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bad Bunny</c:v>
+                  <c:v>Rihanna</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -651,13 +663,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8400000</c:v>
+                  <c:v>46000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43000000</c:v>
+                  <c:v>70000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88000000</c:v>
+                  <c:v>70000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,7 +822,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -967,7 +979,7 @@
               <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
                 <a:ln w="0"/>
                 <a:solidFill>
-                  <a:srgbClr val="00B050"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
                 <a:effectLst>
                   <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
@@ -1666,16 +1678,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2000,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F11A846-44B5-C441-8003-7CB3B4FB2BE5}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2027,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>23000000</v>
+        <v>41400000</v>
       </c>
       <c r="C2">
         <v>80000000</v>
@@ -2041,13 +2053,13 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>49000000</v>
+      </c>
+      <c r="C3">
         <v>14200000</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="1">
         <v>50000000</v>
-      </c>
-      <c r="D3">
-        <v>40000000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2055,13 +2067,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>14700000</v>
+        <v>32800000</v>
       </c>
       <c r="C4">
         <v>75000000</v>
       </c>
       <c r="D4">
-        <v>30000000</v>
+        <v>75000000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2069,10 +2081,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>23200000</v>
+        <v>29700000</v>
       </c>
       <c r="C5">
-        <v>24000000</v>
+        <v>60000000</v>
       </c>
       <c r="D5">
         <v>45000000</v>
@@ -2082,18 +2094,22 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>8400000</v>
-      </c>
-      <c r="C6">
-        <v>43000000</v>
+      <c r="B6" s="1">
+        <v>46000000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>70000000</v>
       </c>
       <c r="D6">
-        <v>88000000</v>
-      </c>
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>